<commit_message>
Updated species list, map centering fix
</commit_message>
<xml_diff>
--- a/scripts/voedselbos_species.xlsx
+++ b/scripts/voedselbos_species.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\map_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11DA0CC-3405-40D0-B759-00901C3C8210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CBB671-BB6A-4A0A-BA23-68E1BD94A7BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1755" yWindow="1170" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
+    <workbookView xWindow="2340" yWindow="840" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="477">
   <si>
     <t>Hovenia dulcis</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Pyrus communis</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Sorbus torminalis</t>
   </si>
   <si>
@@ -96,9 +93,6 @@
     <t>Ballerina</t>
   </si>
   <si>
-    <t>Amelanchier </t>
-  </si>
-  <si>
     <t>Princess Diana, Prince Charles</t>
   </si>
   <si>
@@ -120,9 +114,6 @@
     <t>Chaenomeles cathayensis</t>
   </si>
   <si>
-    <t>Chinese kwee </t>
-  </si>
-  <si>
     <t>Cornus kousa</t>
   </si>
   <si>
@@ -186,15 +177,9 @@
     <t>Gloire de Sabron</t>
   </si>
   <si>
-    <t>Rode bes</t>
-  </si>
-  <si>
     <t>Rubus 'Loganberry'</t>
   </si>
   <si>
-    <t>Framboos</t>
-  </si>
-  <si>
     <t>Rubus phoenicolasius</t>
   </si>
   <si>
@@ -222,12 +207,6 @@
     <t>Maar 1 leverbaar, nog 1 nabestellen</t>
   </si>
   <si>
-    <t>Eetbare lijsterbes</t>
-  </si>
-  <si>
-    <t>Sorbus 'Burka</t>
-  </si>
-  <si>
     <t>Bursinka</t>
   </si>
   <si>
@@ -279,9 +258,6 @@
     <t>Sierkwee</t>
   </si>
   <si>
-    <t>Vaccinium macrocarpum</t>
-  </si>
-  <si>
     <t>Pilgrim</t>
   </si>
   <si>
@@ -327,9 +303,6 @@
     <t>big redd</t>
   </si>
   <si>
-    <t>Crataegus pinnatifida major “Big ball”</t>
-  </si>
-  <si>
     <t>Crataegus schraderiana</t>
   </si>
   <si>
@@ -369,9 +342,6 @@
     <t>Oleaster</t>
   </si>
   <si>
-    <t>Desmodium elegans</t>
-  </si>
-  <si>
     <t>Sambucus canadensis</t>
   </si>
   <si>
@@ -411,18 +381,9 @@
     <t>Aardbeiboom</t>
   </si>
   <si>
-    <t>Eriobotrya japonica </t>
-  </si>
-  <si>
-    <t>Pseudocydonia sinensis </t>
-  </si>
-  <si>
     <t>Chinese kweepeer</t>
   </si>
   <si>
-    <t>Ziziphus jujube</t>
-  </si>
-  <si>
     <t>Lang, zaailing</t>
   </si>
   <si>
@@ -627,9 +588,6 @@
     <t>Brecht, Gwens, Idaho niet voorradig. Later nog 3 bestellen</t>
   </si>
   <si>
-    <t>Buffelkrent</t>
-  </si>
-  <si>
     <t>Rubus 'Tayberry'</t>
   </si>
   <si>
@@ -685,9 +643,6 @@
   </si>
   <si>
     <t>Alba</t>
-  </si>
-  <si>
-    <t>Tilia cordata </t>
   </si>
   <si>
     <t>Alnus incana</t>
@@ -874,9 +829,6 @@
     <t>D. virginiana</t>
   </si>
   <si>
-    <t>Desmodium sp.</t>
-  </si>
-  <si>
     <t>E. angustifolia</t>
   </si>
   <si>
@@ -1201,12 +1153,6 @@
     <t xml:space="preserve">Callicarpa anomala </t>
   </si>
   <si>
-    <t>V. macrocarpum</t>
-  </si>
-  <si>
-    <t>T. cordata </t>
-  </si>
-  <si>
     <t>S. alba</t>
   </si>
   <si>
@@ -1270,15 +1216,6 @@
     <t>Peer (hoogstam)</t>
   </si>
   <si>
-    <t>Bottelroos (rimpelroos)</t>
-  </si>
-  <si>
-    <t>Franseuiensoepboom (geknot)</t>
-  </si>
-  <si>
-    <t>Winterlinde (geknot)</t>
-  </si>
-  <si>
     <t>Fluweelboom (klein)</t>
   </si>
   <si>
@@ -1340,6 +1277,186 @@
   </si>
   <si>
     <t>Kweepeer</t>
+  </si>
+  <si>
+    <t>Chinese jujube</t>
+  </si>
+  <si>
+    <t>Zizyphus jujuba</t>
+  </si>
+  <si>
+    <t>Appel (wilde)</t>
+  </si>
+  <si>
+    <t>Malus sylvestris</t>
+  </si>
+  <si>
+    <t>M. sylvestris</t>
+  </si>
+  <si>
+    <t>Apple (wild)</t>
+  </si>
+  <si>
+    <t>Pepper Tree</t>
+  </si>
+  <si>
+    <t>American cranberry</t>
+  </si>
+  <si>
+    <t>Vaccinium macrocarpon</t>
+  </si>
+  <si>
+    <t>V. macrocarpon</t>
+  </si>
+  <si>
+    <t>Chinese mahogany</t>
+  </si>
+  <si>
+    <t>Winterlinde</t>
+  </si>
+  <si>
+    <t>Franseuiensoepboom</t>
+  </si>
+  <si>
+    <t>Small-leaved linden</t>
+  </si>
+  <si>
+    <t>American bladdernut</t>
+  </si>
+  <si>
+    <t>European bladdernut</t>
+  </si>
+  <si>
+    <t>Service tree</t>
+  </si>
+  <si>
+    <t>Sorbus 'Burka'</t>
+  </si>
+  <si>
+    <t>Schoonvrucht</t>
+  </si>
+  <si>
+    <t>Mountain-ash</t>
+  </si>
+  <si>
+    <t>Lijsterbes</t>
+  </si>
+  <si>
+    <t>Grootvruchtige lijsterbes</t>
+  </si>
+  <si>
+    <t>Silver buffaloberry</t>
+  </si>
+  <si>
+    <t>Elderberry</t>
+  </si>
+  <si>
+    <t>White willow</t>
+  </si>
+  <si>
+    <t>Tayberry</t>
+  </si>
+  <si>
+    <t>Loganberry</t>
+  </si>
+  <si>
+    <t>Frambraam</t>
+  </si>
+  <si>
+    <t>Aardbeiframboos</t>
+  </si>
+  <si>
+    <t>Strawberry raspberry</t>
+  </si>
+  <si>
+    <t>Beach rose</t>
+  </si>
+  <si>
+    <t>Rimpelroos</t>
+  </si>
+  <si>
+    <t>Redcurrant</t>
+  </si>
+  <si>
+    <t>Aalbes</t>
+  </si>
+  <si>
+    <t>Clove currant</t>
+  </si>
+  <si>
+    <t>Gele ribes</t>
+  </si>
+  <si>
+    <t>Staghorn sumac</t>
+  </si>
+  <si>
+    <t>Gooseberry</t>
+  </si>
+  <si>
+    <t>Smooth sumac</t>
+  </si>
+  <si>
+    <t>Fragrant sumac</t>
+  </si>
+  <si>
+    <t>Holm oak</t>
+  </si>
+  <si>
+    <t>European pear</t>
+  </si>
+  <si>
+    <t>Chinese quince</t>
+  </si>
+  <si>
+    <t>Rowan</t>
+  </si>
+  <si>
+    <t>Sour cherry</t>
+  </si>
+  <si>
+    <t>Plum</t>
+  </si>
+  <si>
+    <t>Cornelian cherry</t>
+  </si>
+  <si>
+    <t>Picea</t>
+  </si>
+  <si>
+    <t>Spar</t>
+  </si>
+  <si>
+    <t>Willow</t>
+  </si>
+  <si>
+    <t>Wilg</t>
+  </si>
+  <si>
+    <t>Salix</t>
+  </si>
+  <si>
+    <t>Crataegus</t>
+  </si>
+  <si>
+    <t>Tilia cordata</t>
+  </si>
+  <si>
+    <t>T. cordata</t>
+  </si>
+  <si>
+    <t>Pseudocydonia sinensis</t>
+  </si>
+  <si>
+    <t>Eriobotrya japonica</t>
+  </si>
+  <si>
+    <t>Crataegus pinnatifida major</t>
+  </si>
+  <si>
+    <t>Chinese kwee</t>
+  </si>
+  <si>
+    <t>Spruce</t>
   </si>
 </sst>
 </file>
@@ -1698,17 +1815,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280D093D-8C82-4BD1-88A3-14D709597181}">
-  <dimension ref="A1:G123"/>
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="87.140625" customWidth="1"/>
@@ -1716,238 +1834,253 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="B1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="C1" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="D1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="E1" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="F1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="G1" t="s">
-        <v>409</v>
+        <v>391</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>343</v>
+        <v>370</v>
+      </c>
+      <c r="D2" t="s">
+        <v>371</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>2.5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>219</v>
       </c>
       <c r="C3" t="s">
-        <v>386</v>
-      </c>
-      <c r="D3" t="s">
-        <v>387</v>
+        <v>220</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F3">
-        <v>2.5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>389</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="E4">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>3.5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>206</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>366</v>
+        <v>327</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>3.5</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>407</v>
+        <v>235</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="E6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>248</v>
+        <v>330</v>
       </c>
       <c r="B7" t="s">
-        <v>234</v>
+        <v>343</v>
       </c>
       <c r="C7" t="s">
-        <v>235</v>
+        <v>341</v>
+      </c>
+      <c r="D7" t="s">
+        <v>342</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B8" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="C8" t="s">
-        <v>127</v>
-      </c>
-      <c r="D8" t="s">
-        <v>389</v>
+        <v>328</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F8">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>406</v>
+        <v>236</v>
       </c>
       <c r="B9" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>174</v>
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>373</v>
       </c>
       <c r="E9">
-        <v>0.25</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>0.25</v>
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>346</v>
+        <v>388</v>
       </c>
       <c r="B10" t="s">
-        <v>359</v>
+        <v>160</v>
       </c>
       <c r="C10" t="s">
-        <v>357</v>
-      </c>
-      <c r="D10" t="s">
-        <v>358</v>
+        <v>161</v>
+      </c>
+      <c r="E10">
+        <v>0.25</v>
+      </c>
+      <c r="F10">
+        <v>0.25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>234</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>234</v>
       </c>
       <c r="C11" t="s">
-        <v>422</v>
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>350</v>
       </c>
       <c r="E11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>252</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>226</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>180</v>
+        <v>401</v>
       </c>
       <c r="E12">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="F12">
-        <v>2.5</v>
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="B13" t="s">
-        <v>181</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E13">
         <v>2.5</v>
@@ -1955,356 +2088,359 @@
       <c r="F13">
         <v>2.5</v>
       </c>
-      <c r="G13" t="s">
-        <v>182</v>
-      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="B14" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="G14" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>405</v>
+        <v>242</v>
       </c>
       <c r="B15" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="C15" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
       <c r="E15">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>257</v>
+        <v>387</v>
       </c>
       <c r="B16" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="E16">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F16">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>347</v>
+        <v>239</v>
       </c>
       <c r="B17" t="s">
-        <v>390</v>
-      </c>
-      <c r="D17" t="s">
-        <v>379</v>
+        <v>165</v>
+      </c>
+      <c r="C17" t="s">
+        <v>167</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>404</v>
+        <v>331</v>
       </c>
       <c r="B18" t="s">
-        <v>213</v>
+        <v>374</v>
       </c>
       <c r="C18" t="s">
-        <v>214</v>
+        <v>435</v>
+      </c>
+      <c r="D18" t="s">
+        <v>363</v>
       </c>
       <c r="E18">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F18">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>264</v>
+        <v>386</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>199</v>
       </c>
       <c r="C19" t="s">
-        <v>159</v>
+        <v>200</v>
       </c>
       <c r="E19">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F19">
-        <v>15</v>
-      </c>
-      <c r="G19" t="s">
-        <v>158</v>
+        <v>4</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>333</v>
       </c>
       <c r="E20">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F20">
-        <v>20</v>
-      </c>
-      <c r="G20" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>408</v>
+        <v>244</v>
       </c>
       <c r="B21" t="s">
-        <v>241</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>225</v>
+      </c>
+      <c r="D21" t="s">
+        <v>345</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F21">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="G21" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>403</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s">
-        <v>175</v>
+        <v>94</v>
       </c>
       <c r="C22" t="s">
-        <v>177</v>
+        <v>89</v>
+      </c>
+      <c r="D22" t="s">
+        <v>333</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="F22">
-        <v>3</v>
-      </c>
-      <c r="G22" t="s">
-        <v>176</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>154</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>362</v>
       </c>
       <c r="E23">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F23">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>247</v>
       </c>
       <c r="B24" t="s">
-        <v>204</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>373</v>
-      </c>
-      <c r="D24" t="s">
-        <v>369</v>
+        <v>475</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>205</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="B25" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>372</v>
+        <v>333</v>
       </c>
       <c r="E25">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>277</v>
+        <v>390</v>
       </c>
       <c r="B26" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C26" t="s">
-        <v>371</v>
-      </c>
-      <c r="D26" t="s">
-        <v>370</v>
+        <v>69</v>
       </c>
       <c r="E26">
-        <v>1.5</v>
+        <v>10</v>
       </c>
       <c r="F26">
-        <v>1.5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>233</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>270</v>
+        <v>385</v>
       </c>
       <c r="B27" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
-        <v>185</v>
-      </c>
-      <c r="D27" t="s">
-        <v>348</v>
+        <v>164</v>
       </c>
       <c r="E27">
         <v>3</v>
       </c>
       <c r="F27">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>266</v>
+        <v>249</v>
       </c>
       <c r="B28" t="s">
-        <v>32</v>
+        <v>144</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>146</v>
       </c>
       <c r="D28" t="s">
-        <v>360</v>
+        <v>146</v>
       </c>
       <c r="E28">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="F28">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>33</v>
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>267</v>
+        <v>250</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>357</v>
+      </c>
+      <c r="D29" t="s">
+        <v>353</v>
       </c>
       <c r="E29">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="B30" t="s">
-        <v>238</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>240</v>
+        <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="E30">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F30">
         <v>6</v>
       </c>
       <c r="G30" t="s">
-        <v>239</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>147</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="D31" t="s">
-        <v>349</v>
+        <v>463</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -2312,42 +2448,45 @@
       <c r="F31">
         <v>5</v>
       </c>
+      <c r="G31" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="B32" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E32">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F32">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>261</v>
+        <v>415</v>
       </c>
       <c r="B33" t="s">
-        <v>167</v>
+        <v>414</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>416</v>
       </c>
       <c r="D33" t="s">
-        <v>378</v>
+        <v>356</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -2355,125 +2494,125 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
         <v>6</v>
       </c>
-      <c r="F34">
-        <v>5</v>
-      </c>
       <c r="G34" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
       <c r="B35" t="s">
-        <v>102</v>
+        <v>170</v>
       </c>
       <c r="C35" t="s">
-        <v>97</v>
+        <v>172</v>
       </c>
       <c r="D35" t="s">
-        <v>349</v>
+        <v>332</v>
       </c>
       <c r="E35">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="G35" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="B36" t="s">
-        <v>98</v>
+        <v>150</v>
       </c>
       <c r="C36" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E36">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F36">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>99</v>
+        <v>151</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="B37" t="s">
-        <v>163</v>
+        <v>474</v>
       </c>
       <c r="C37" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E37">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F37">
-        <v>5</v>
-      </c>
-      <c r="G37" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="B38" t="s">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" t="s">
-        <v>349</v>
+        <v>27</v>
       </c>
       <c r="E38">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F38">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="G38" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="B39" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C39" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -2484,112 +2623,136 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>276</v>
+        <v>384</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>13</v>
       </c>
       <c r="C40" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" t="s">
-        <v>349</v>
+        <v>14</v>
       </c>
       <c r="E40">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F40">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>400</v>
+        <v>260</v>
       </c>
       <c r="B41" t="s">
-        <v>136</v>
+        <v>74</v>
       </c>
       <c r="C41" t="s">
-        <v>138</v>
+        <v>76</v>
+      </c>
+      <c r="D41" t="s">
+        <v>356</v>
       </c>
       <c r="E41">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F41">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G41" t="s">
-        <v>137</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>401</v>
+        <v>261</v>
       </c>
       <c r="B42" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="C42" t="s">
-        <v>17</v>
+        <v>89</v>
+      </c>
+      <c r="D42" t="s">
+        <v>333</v>
       </c>
       <c r="E42">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>402</v>
+        <v>382</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
       <c r="C43" t="s">
-        <v>15</v>
+        <v>125</v>
       </c>
       <c r="E43">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="G43" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="B44" t="s">
-        <v>92</v>
+        <v>217</v>
       </c>
       <c r="C44" t="s">
-        <v>412</v>
+        <v>355</v>
+      </c>
+      <c r="D44" t="s">
+        <v>354</v>
       </c>
       <c r="E44">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>282</v>
+        <v>383</v>
       </c>
       <c r="B45" t="s">
-        <v>114</v>
+        <v>15</v>
+      </c>
+      <c r="C45" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>279</v>
+        <v>469</v>
       </c>
       <c r="B46" t="s">
-        <v>93</v>
+        <v>469</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>89</v>
+      </c>
+      <c r="D46" t="s">
+        <v>333</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -2600,93 +2763,87 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>281</v>
+        <v>263</v>
       </c>
       <c r="B47" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>141</v>
+        <v>394</v>
       </c>
       <c r="E47">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="F47">
-        <v>10</v>
-      </c>
-      <c r="G47" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="B48" t="s">
-        <v>142</v>
+        <v>85</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>86</v>
       </c>
       <c r="E48">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F48">
-        <v>8</v>
-      </c>
-      <c r="G48" t="s">
-        <v>143</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>283</v>
+        <v>265</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C49" t="s">
-        <v>113</v>
+        <v>131</v>
       </c>
       <c r="E49">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>8</v>
+      </c>
+      <c r="G49" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="B50" t="s">
-        <v>229</v>
+        <v>126</v>
       </c>
       <c r="C50" t="s">
-        <v>231</v>
+        <v>128</v>
       </c>
       <c r="E50">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>230</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>285</v>
+        <v>267</v>
       </c>
       <c r="B51" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C51" t="s">
-        <v>108</v>
-      </c>
-      <c r="D51" t="s">
-        <v>353</v>
+        <v>104</v>
       </c>
       <c r="E51">
         <v>3</v>
@@ -2694,22 +2851,19 @@
       <c r="F51">
         <v>3</v>
       </c>
-      <c r="G51" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>399</v>
+        <v>268</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>473</v>
       </c>
       <c r="C52" t="s">
-        <v>118</v>
+        <v>393</v>
       </c>
       <c r="E52">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F52">
         <v>5</v>
@@ -2717,161 +2871,170 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="B53" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>411</v>
+        <v>99</v>
+      </c>
+      <c r="D53" t="s">
+        <v>337</v>
       </c>
       <c r="E53">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F53">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="G53" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>256</v>
+        <v>381</v>
       </c>
       <c r="B54" t="s">
-        <v>186</v>
+        <v>107</v>
       </c>
       <c r="C54" t="s">
-        <v>344</v>
+        <v>108</v>
       </c>
       <c r="E54">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F54">
-        <v>3</v>
-      </c>
-      <c r="G54" t="s">
-        <v>187</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>287</v>
+        <v>270</v>
       </c>
       <c r="B55" t="s">
-        <v>35</v>
+        <v>214</v>
       </c>
       <c r="C55" t="s">
-        <v>345</v>
+        <v>216</v>
       </c>
       <c r="E55">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F55">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>36</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>288</v>
+        <v>379</v>
       </c>
       <c r="B56" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="C56" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
       <c r="E56">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>289</v>
+        <v>271</v>
       </c>
       <c r="B57" t="s">
-        <v>190</v>
+        <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>192</v>
+        <v>329</v>
       </c>
       <c r="E57">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G57" t="s">
-        <v>191</v>
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>397</v>
+        <v>413</v>
       </c>
       <c r="B58" t="s">
-        <v>224</v>
+        <v>412</v>
       </c>
       <c r="C58" t="s">
-        <v>225</v>
+        <v>410</v>
+      </c>
+      <c r="D58" t="s">
+        <v>411</v>
+      </c>
+      <c r="E58">
+        <v>14</v>
+      </c>
+      <c r="F58">
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>398</v>
+        <v>272</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="C59" t="s">
-        <v>420</v>
-      </c>
-      <c r="D59" t="s">
-        <v>419</v>
+        <v>176</v>
       </c>
       <c r="E59">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="F59">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>290</v>
+        <v>273</v>
       </c>
       <c r="B60" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="C60" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="E60">
-        <v>10</v>
+        <v>2.5</v>
       </c>
       <c r="F60">
-        <v>10</v>
+        <v>2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>291</v>
+        <v>274</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C61" t="s">
-        <v>194</v>
-      </c>
-      <c r="D61" t="s">
-        <v>355</v>
+        <v>196</v>
       </c>
       <c r="E61">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F61">
         <v>10</v>
@@ -2879,13 +3042,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>292</v>
+        <v>380</v>
       </c>
       <c r="B62" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>78</v>
+        <v>399</v>
+      </c>
+      <c r="D62" t="s">
+        <v>398</v>
       </c>
       <c r="E62">
         <v>1.5</v>
@@ -2896,47 +3062,50 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>293</v>
+        <v>275</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>181</v>
+      </c>
+      <c r="D63" t="s">
+        <v>339</v>
       </c>
       <c r="E63">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F63">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>12</v>
+        <v>276</v>
       </c>
       <c r="B64" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
+        <v>71</v>
       </c>
       <c r="E64">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F64">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>396</v>
+        <v>277</v>
       </c>
       <c r="B65" t="s">
-        <v>215</v>
+        <v>34</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>35</v>
       </c>
       <c r="E65">
         <v>6</v>
@@ -2944,19 +3113,16 @@
       <c r="F65">
         <v>5</v>
       </c>
-      <c r="G65" t="s">
-        <v>216</v>
-      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="E66">
         <v>10</v>
@@ -2967,90 +3133,90 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>295</v>
+        <v>378</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C67" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="E67">
-        <v>2.5</v>
+        <v>6</v>
       </c>
       <c r="F67">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="G67" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>300</v>
+      <c r="A68" t="s">
+        <v>11</v>
       </c>
       <c r="B68" t="s">
-        <v>410</v>
+        <v>11</v>
       </c>
       <c r="C68" t="s">
-        <v>228</v>
+        <v>12</v>
       </c>
       <c r="E68">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="F68">
-        <v>7</v>
-      </c>
-      <c r="G68" t="s">
-        <v>75</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>297</v>
+        <v>407</v>
       </c>
       <c r="B69" t="s">
-        <v>227</v>
+        <v>406</v>
       </c>
       <c r="C69" t="s">
-        <v>228</v>
+        <v>409</v>
+      </c>
+      <c r="D69" t="s">
+        <v>408</v>
       </c>
       <c r="E69">
+        <v>30</v>
+      </c>
+      <c r="F69">
         <v>10</v>
-      </c>
-      <c r="F69">
-        <v>7</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>298</v>
+        <v>279</v>
       </c>
       <c r="B70" t="s">
-        <v>109</v>
+        <v>182</v>
       </c>
       <c r="C70" t="s">
-        <v>111</v>
+        <v>184</v>
       </c>
       <c r="E70">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="F70">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="G70" t="s">
-        <v>110</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="B71" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="E71">
         <v>15</v>
@@ -3059,149 +3225,158 @@
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>299</v>
+      <c r="A72" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="B72" t="s">
-        <v>151</v>
+        <v>392</v>
       </c>
       <c r="C72" t="s">
-        <v>153</v>
+        <v>213</v>
       </c>
       <c r="E72">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="F72">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G72" t="s">
-        <v>152</v>
+        <v>68</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>212</v>
       </c>
       <c r="C73" t="s">
-        <v>150</v>
+        <v>213</v>
       </c>
       <c r="E73">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F73">
-        <v>10</v>
-      </c>
-      <c r="G73" t="s">
-        <v>149</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>362</v>
+        <v>282</v>
       </c>
       <c r="B74" t="s">
-        <v>365</v>
+        <v>100</v>
       </c>
       <c r="C74" t="s">
-        <v>363</v>
-      </c>
-      <c r="D74" t="s">
-        <v>364</v>
+        <v>102</v>
+      </c>
+      <c r="E74">
+        <v>5</v>
+      </c>
+      <c r="F74">
+        <v>4</v>
+      </c>
+      <c r="G74" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>242</v>
+        <v>283</v>
       </c>
       <c r="B75" t="s">
-        <v>242</v>
+        <v>138</v>
       </c>
       <c r="C75" t="s">
-        <v>243</v>
+        <v>140</v>
       </c>
       <c r="E75">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="F75">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="G75" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>306</v>
+        <v>346</v>
       </c>
       <c r="B76" t="s">
-        <v>39</v>
+        <v>349</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>347</v>
+      </c>
+      <c r="D76" t="s">
+        <v>348</v>
       </c>
       <c r="E76">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F76">
-        <v>15</v>
-      </c>
-      <c r="G76" t="s">
-        <v>40</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="B77" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C77" t="s">
-        <v>170</v>
-      </c>
-      <c r="D77" t="s">
-        <v>354</v>
+        <v>137</v>
       </c>
       <c r="E77">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F77">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>308</v>
+        <v>421</v>
       </c>
       <c r="B78" t="s">
-        <v>244</v>
+        <v>420</v>
       </c>
       <c r="C78" t="s">
-        <v>244</v>
+        <v>419</v>
       </c>
       <c r="D78" t="s">
-        <v>244</v>
+        <v>422</v>
+      </c>
+      <c r="E78">
+        <v>6</v>
+      </c>
+      <c r="F78">
+        <v>4</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
       <c r="B79" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C79" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D79" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="E79">
         <v>6</v>
@@ -3210,18 +3385,21 @@
         <v>4</v>
       </c>
       <c r="G79" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="B80" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C80" t="s">
-        <v>135</v>
+        <v>122</v>
+      </c>
+      <c r="D80" t="s">
+        <v>461</v>
       </c>
       <c r="E80">
         <v>4</v>
@@ -3230,274 +3408,313 @@
         <v>4</v>
       </c>
       <c r="G80" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>305</v>
+        <v>288</v>
       </c>
       <c r="B81" t="s">
-        <v>122</v>
+        <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>124</v>
+        <v>395</v>
+      </c>
+      <c r="D81" t="s">
+        <v>458</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F81">
-        <v>3</v>
-      </c>
-      <c r="G81" t="s">
-        <v>123</v>
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>309</v>
+        <v>289</v>
       </c>
       <c r="B82" t="s">
-        <v>245</v>
+        <v>112</v>
       </c>
       <c r="C82" t="s">
-        <v>246</v>
+        <v>114</v>
       </c>
       <c r="D82" t="s">
-        <v>388</v>
+        <v>462</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82">
+        <v>3</v>
+      </c>
+      <c r="G82" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>310</v>
+        <v>290</v>
       </c>
       <c r="B83" t="s">
-        <v>129</v>
+        <v>36</v>
       </c>
       <c r="C83" t="s">
-        <v>130</v>
+        <v>38</v>
       </c>
       <c r="E83">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="F83">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="G83" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="B84" t="s">
-        <v>1</v>
+        <v>155</v>
       </c>
       <c r="C84" t="s">
-        <v>413</v>
+        <v>157</v>
+      </c>
+      <c r="D84" t="s">
+        <v>338</v>
       </c>
       <c r="E84">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F84">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>2</v>
+        <v>156</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>311</v>
+        <v>292</v>
       </c>
       <c r="B85" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="C85" t="s">
-        <v>166</v>
+        <v>229</v>
+      </c>
+      <c r="D85" t="s">
+        <v>229</v>
+      </c>
+      <c r="E85">
+        <v>5</v>
+      </c>
+      <c r="F85">
+        <v>3</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>314</v>
+        <v>293</v>
       </c>
       <c r="B86" t="s">
-        <v>42</v>
+        <v>230</v>
       </c>
       <c r="C86" t="s">
-        <v>417</v>
+        <v>231</v>
+      </c>
+      <c r="D86" t="s">
+        <v>372</v>
       </c>
       <c r="E86">
-        <v>1.5</v>
+        <v>8</v>
       </c>
       <c r="F86">
-        <v>1.5</v>
-      </c>
-      <c r="G86" t="s">
-        <v>43</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>316</v>
+        <v>294</v>
       </c>
       <c r="B87" t="s">
-        <v>44</v>
+        <v>472</v>
       </c>
       <c r="C87" t="s">
-        <v>45</v>
+        <v>118</v>
+      </c>
+      <c r="D87" t="s">
+        <v>459</v>
       </c>
       <c r="E87">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F87">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>321</v>
+        <v>227</v>
       </c>
       <c r="B88" t="s">
-        <v>90</v>
+        <v>227</v>
       </c>
       <c r="C88" t="s">
-        <v>45</v>
+        <v>228</v>
       </c>
       <c r="E88">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F88">
-        <v>3</v>
-      </c>
-      <c r="G88" t="s">
-        <v>91</v>
+        <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>315</v>
+        <v>464</v>
       </c>
       <c r="B89" t="s">
-        <v>46</v>
+        <v>464</v>
       </c>
       <c r="C89" t="s">
-        <v>47</v>
+        <v>465</v>
+      </c>
+      <c r="D89" t="s">
+        <v>476</v>
       </c>
       <c r="E89">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="F89">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="B90" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="C90" t="s">
-        <v>50</v>
+        <v>153</v>
       </c>
       <c r="D90" t="s">
-        <v>350</v>
+        <v>457</v>
       </c>
       <c r="E90">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F90">
-        <v>1.5</v>
-      </c>
-      <c r="G90" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>319</v>
+        <v>296</v>
       </c>
       <c r="B91" t="s">
-        <v>198</v>
+        <v>50</v>
       </c>
       <c r="C91" t="s">
-        <v>200</v>
+        <v>444</v>
+      </c>
+      <c r="D91" t="s">
+        <v>443</v>
       </c>
       <c r="E91">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="F91">
-        <v>1.25</v>
-      </c>
-      <c r="G91" t="s">
-        <v>199</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="B92" t="s">
-        <v>51</v>
+        <v>187</v>
       </c>
       <c r="C92" t="s">
-        <v>53</v>
+        <v>189</v>
+      </c>
+      <c r="D92" t="s">
+        <v>442</v>
       </c>
       <c r="E92">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F92">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G92" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>395</v>
+        <v>298</v>
       </c>
       <c r="B93" t="s">
-        <v>218</v>
+        <v>39</v>
       </c>
       <c r="C93" t="s">
-        <v>414</v>
+        <v>396</v>
+      </c>
+      <c r="D93" t="s">
+        <v>456</v>
       </c>
       <c r="E93">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F93">
         <v>1.5</v>
       </c>
       <c r="G93" t="s">
-        <v>219</v>
+        <v>40</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>317</v>
+        <v>299</v>
       </c>
       <c r="B94" t="s">
-        <v>10</v>
+        <v>43</v>
+      </c>
+      <c r="C94" t="s">
+        <v>44</v>
+      </c>
+      <c r="D94" t="s">
+        <v>454</v>
       </c>
       <c r="E94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="B95" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C95" t="s">
-        <v>55</v>
+        <v>42</v>
+      </c>
+      <c r="D95" t="s">
+        <v>455</v>
       </c>
       <c r="E95">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -3505,543 +3722,669 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>394</v>
+        <v>301</v>
       </c>
       <c r="B96" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>377</v>
+        <v>445</v>
       </c>
       <c r="D96" t="s">
-        <v>376</v>
+        <v>446</v>
       </c>
       <c r="E96">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F96">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>421</v>
+        <v>376</v>
       </c>
       <c r="B97" t="s">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="C97" t="s">
-        <v>57</v>
+        <v>361</v>
       </c>
       <c r="D97" t="s">
-        <v>375</v>
+        <v>360</v>
       </c>
       <c r="E97">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B98" t="s">
-        <v>201</v>
+        <v>45</v>
       </c>
       <c r="C98" t="s">
-        <v>203</v>
+        <v>47</v>
+      </c>
+      <c r="D98" t="s">
+        <v>334</v>
       </c>
       <c r="E98">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F98">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G98" t="s">
-        <v>202</v>
+        <v>46</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>393</v>
+        <v>303</v>
       </c>
       <c r="B99" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="C99" t="s">
-        <v>223</v>
+        <v>452</v>
+      </c>
+      <c r="D99" t="s">
+        <v>451</v>
+      </c>
+      <c r="E99">
+        <v>1.25</v>
+      </c>
+      <c r="F99">
+        <v>1.25</v>
+      </c>
+      <c r="G99" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>324</v>
+        <v>400</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>51</v>
       </c>
       <c r="C100" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="D100" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E100">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F100">
-        <v>2.5</v>
-      </c>
-      <c r="G100" t="s">
-        <v>116</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>326</v>
+        <v>304</v>
       </c>
       <c r="B101" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C101" t="s">
-        <v>60</v>
+        <v>450</v>
+      </c>
+      <c r="D101" t="s">
+        <v>449</v>
       </c>
       <c r="E101">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F101">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G101" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>322</v>
+        <v>377</v>
       </c>
       <c r="B102" t="s">
-        <v>61</v>
+        <v>204</v>
       </c>
       <c r="C102" t="s">
-        <v>62</v>
+        <v>448</v>
+      </c>
+      <c r="D102" t="s">
+        <v>447</v>
       </c>
       <c r="E102">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F102">
-        <v>3</v>
+        <v>1.5</v>
+      </c>
+      <c r="G102" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>323</v>
+        <v>305</v>
       </c>
       <c r="B103" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
       <c r="C103" t="s">
-        <v>65</v>
+        <v>42</v>
+      </c>
+      <c r="D103" t="s">
+        <v>453</v>
       </c>
       <c r="E103">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F103">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G103" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>330</v>
+        <v>403</v>
       </c>
       <c r="B104" t="s">
-        <v>66</v>
+        <v>402</v>
+      </c>
+      <c r="C104" t="s">
+        <v>404</v>
+      </c>
+      <c r="D104" t="s">
+        <v>405</v>
       </c>
       <c r="E104">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F104">
-        <v>5</v>
-      </c>
-      <c r="G104" t="s">
-        <v>67</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>325</v>
+        <v>375</v>
       </c>
       <c r="B105" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="C105" t="s">
-        <v>156</v>
+        <v>208</v>
+      </c>
+      <c r="D105" t="s">
+        <v>441</v>
       </c>
       <c r="E105">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F105">
-        <v>8</v>
-      </c>
-      <c r="G105" t="s">
-        <v>155</v>
+        <v>10</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>328</v>
+        <v>306</v>
       </c>
       <c r="B106" t="s">
+        <v>56</v>
+      </c>
+      <c r="C106" t="s">
+        <v>57</v>
+      </c>
+      <c r="D106" t="s">
+        <v>439</v>
+      </c>
+      <c r="E106">
+        <v>4</v>
+      </c>
+      <c r="F106">
         <v>3</v>
-      </c>
-      <c r="C106" t="s">
-        <v>4</v>
-      </c>
-      <c r="D106" t="s">
-        <v>356</v>
-      </c>
-      <c r="E106">
-        <v>20</v>
-      </c>
-      <c r="F106">
-        <v>8</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>327</v>
+        <v>307</v>
       </c>
       <c r="B107" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C107" t="s">
-        <v>69</v>
+        <v>438</v>
+      </c>
+      <c r="D107" t="s">
+        <v>460</v>
       </c>
       <c r="E107">
-        <v>43224</v>
+        <v>12</v>
       </c>
       <c r="F107">
-        <v>43224</v>
+        <v>7</v>
+      </c>
+      <c r="G107" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>329</v>
+        <v>308</v>
       </c>
       <c r="B108" t="s">
-        <v>206</v>
+        <v>105</v>
       </c>
       <c r="C108" t="s">
-        <v>208</v>
+        <v>55</v>
+      </c>
+      <c r="D108" t="s">
+        <v>351</v>
       </c>
       <c r="E108">
         <v>3</v>
       </c>
       <c r="F108">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="G108" t="s">
-        <v>207</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>392</v>
+        <v>309</v>
       </c>
       <c r="B109" t="s">
-        <v>220</v>
+        <v>141</v>
       </c>
       <c r="C109" t="s">
-        <v>416</v>
+        <v>143</v>
+      </c>
+      <c r="D109" t="s">
+        <v>433</v>
       </c>
       <c r="E109">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F109">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="G109" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>332</v>
+        <v>310</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>53</v>
       </c>
       <c r="C110" t="s">
-        <v>415</v>
+        <v>55</v>
+      </c>
+      <c r="D110" t="s">
+        <v>440</v>
       </c>
       <c r="E110">
+        <v>4</v>
+      </c>
+      <c r="F110">
         <v>3</v>
       </c>
-      <c r="F110">
-        <v>2</v>
+      <c r="G110" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>331</v>
+        <v>311</v>
       </c>
       <c r="B111" t="s">
-        <v>6</v>
+        <v>61</v>
       </c>
       <c r="C111" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="D111" t="s">
-        <v>368</v>
+        <v>432</v>
       </c>
       <c r="E111">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F111">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>333</v>
+        <v>312</v>
       </c>
       <c r="B112" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="C112" t="s">
-        <v>80</v>
+        <v>3</v>
+      </c>
+      <c r="D112" t="s">
+        <v>340</v>
       </c>
       <c r="E112">
-        <v>1.5</v>
+        <v>20</v>
       </c>
       <c r="F112">
-        <v>1.5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>391</v>
+        <v>313</v>
       </c>
       <c r="B113" t="s">
-        <v>84</v>
+        <v>192</v>
       </c>
       <c r="C113" t="s">
-        <v>86</v>
+        <v>194</v>
+      </c>
+      <c r="D113" t="s">
+        <v>431</v>
       </c>
       <c r="E113">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="F113">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="G113" t="s">
-        <v>85</v>
+        <v>193</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>381</v>
+        <v>468</v>
       </c>
       <c r="B114" t="s">
-        <v>171</v>
+        <v>468</v>
       </c>
       <c r="C114" t="s">
-        <v>384</v>
+        <v>467</v>
       </c>
       <c r="D114" t="s">
-        <v>385</v>
+        <v>466</v>
       </c>
       <c r="E114">
-        <v>0.5</v>
+        <v>10</v>
       </c>
       <c r="F114">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>380</v>
+        <v>314</v>
       </c>
       <c r="B115" t="s">
-        <v>172</v>
+        <v>434</v>
       </c>
       <c r="C115" t="s">
-        <v>383</v>
+        <v>437</v>
       </c>
       <c r="D115" t="s">
-        <v>382</v>
+        <v>436</v>
       </c>
       <c r="E115">
-        <v>0.2</v>
+        <v>7</v>
       </c>
       <c r="F115">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="G115" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>335</v>
+        <v>471</v>
       </c>
       <c r="B116" t="s">
-        <v>70</v>
+        <v>470</v>
       </c>
       <c r="C116" t="s">
-        <v>71</v>
+        <v>428</v>
       </c>
       <c r="D116" t="s">
-        <v>351</v>
+        <v>430</v>
       </c>
       <c r="E116">
+        <v>3</v>
+      </c>
+      <c r="F116">
         <v>2</v>
-      </c>
-      <c r="F116">
-        <v>1.5</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>336</v>
+        <v>315</v>
       </c>
       <c r="B117" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C117" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D117" t="s">
-        <v>374</v>
+        <v>352</v>
       </c>
       <c r="E117">
-        <v>2.5</v>
+        <v>20</v>
       </c>
       <c r="F117">
-        <v>2.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>72</v>
+        <v>316</v>
       </c>
       <c r="B118" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C118" t="s">
-        <v>74</v>
+        <v>429</v>
+      </c>
+      <c r="D118" t="s">
+        <v>427</v>
       </c>
       <c r="E118">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F118">
         <v>2</v>
       </c>
-      <c r="G118" t="s">
-        <v>73</v>
-      </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>334</v>
+        <v>317</v>
       </c>
       <c r="B119" t="s">
-        <v>131</v>
+        <v>72</v>
       </c>
       <c r="C119" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="D119" t="s">
+        <v>72</v>
       </c>
       <c r="E119">
-        <v>10</v>
+        <v>1.5</v>
       </c>
       <c r="F119">
-        <v>7</v>
-      </c>
-      <c r="G119" t="s">
-        <v>132</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
+        <v>426</v>
+      </c>
+      <c r="B120" t="s">
+        <v>425</v>
+      </c>
+      <c r="C120" t="s">
+        <v>78</v>
+      </c>
+      <c r="D120" t="s">
         <v>424</v>
       </c>
-      <c r="B120" t="s">
-        <v>423</v>
-      </c>
-      <c r="C120" t="s">
-        <v>425</v>
-      </c>
-      <c r="D120" t="s">
-        <v>426</v>
-      </c>
       <c r="E120">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F120">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="G120" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>428</v>
+        <v>365</v>
       </c>
       <c r="B121" t="s">
-        <v>427</v>
+        <v>158</v>
       </c>
       <c r="C121" t="s">
-        <v>430</v>
+        <v>368</v>
       </c>
       <c r="D121" t="s">
-        <v>429</v>
+        <v>369</v>
       </c>
       <c r="E121">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="F121">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>434</v>
+        <v>364</v>
       </c>
       <c r="B122" t="s">
-        <v>433</v>
+        <v>159</v>
       </c>
       <c r="C122" t="s">
-        <v>431</v>
+        <v>367</v>
       </c>
       <c r="D122" t="s">
-        <v>432</v>
+        <v>366</v>
       </c>
       <c r="E122">
-        <v>14</v>
+        <v>0.2</v>
       </c>
       <c r="F122">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>436</v>
+        <v>318</v>
       </c>
       <c r="B123" t="s">
-        <v>435</v>
+        <v>418</v>
       </c>
       <c r="C123" t="s">
-        <v>437</v>
+        <v>417</v>
       </c>
       <c r="D123" t="s">
-        <v>372</v>
+        <v>417</v>
       </c>
       <c r="E123">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="F123">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="G123" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>319</v>
+      </c>
+      <c r="B124" t="s">
+        <v>63</v>
+      </c>
+      <c r="C124" t="s">
+        <v>64</v>
+      </c>
+      <c r="D124" t="s">
+        <v>335</v>
+      </c>
+      <c r="E124">
+        <v>2</v>
+      </c>
+      <c r="F124">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>320</v>
+      </c>
+      <c r="B125" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s">
+        <v>8</v>
+      </c>
+      <c r="D125" t="s">
+        <v>358</v>
+      </c>
+      <c r="E125">
+        <v>2.5</v>
+      </c>
+      <c r="F125">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>65</v>
+      </c>
+      <c r="B126" t="s">
+        <v>65</v>
+      </c>
+      <c r="C126" t="s">
+        <v>67</v>
+      </c>
+      <c r="D126" t="s">
+        <v>423</v>
+      </c>
+      <c r="E126">
+        <v>2</v>
+      </c>
+      <c r="F126">
+        <v>2</v>
+      </c>
+      <c r="G126" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G119">
-    <sortCondition ref="B2:B119"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G126">
+    <sortCondition ref="A2:A126"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated species, added missing English names
</commit_message>
<xml_diff>
--- a/scripts/voedselbos_species.xlsx
+++ b/scripts/voedselbos_species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B28C8B-951D-4EA3-9945-0B9B72E66DC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651B2011-4676-482A-A105-671990386CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="840" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
+    <workbookView xWindow="29010" yWindow="1980" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="520">
   <si>
     <t>Hovenia dulcis</t>
   </si>
@@ -357,9 +357,6 @@
     <t>Early river, Burlat</t>
   </si>
   <si>
-    <t>Zoete kers</t>
-  </si>
-  <si>
     <t>Prunus domestica</t>
   </si>
   <si>
@@ -387,9 +384,6 @@
     <t>Rheinische schattenmorelle</t>
   </si>
   <si>
-    <t>Zure kers</t>
-  </si>
-  <si>
     <t>Cudrania tricuspidata</t>
   </si>
   <si>
@@ -696,9 +690,6 @@
     <t>Cephalotaxus fortunei</t>
   </si>
   <si>
-    <t>Phyllostachis sp.</t>
-  </si>
-  <si>
     <t>Bamboe</t>
   </si>
   <si>
@@ -1155,9 +1146,6 @@
     <t>C. tricuspidata</t>
   </si>
   <si>
-    <t>C.cardunculus</t>
-  </si>
-  <si>
     <t>C. scolymus</t>
   </si>
   <si>
@@ -1185,9 +1173,6 @@
     <t>Mahonia aquifolium</t>
   </si>
   <si>
-    <t>Japanse Wolmispel (Loquat)</t>
-  </si>
-  <si>
     <t>Augurkenstruik (Blauwe boon)</t>
   </si>
   <si>
@@ -1257,9 +1242,6 @@
     <t>Chinese jujube</t>
   </si>
   <si>
-    <t>Zizyphus jujuba</t>
-  </si>
-  <si>
     <t>Appel (wilde)</t>
   </si>
   <si>
@@ -1395,9 +1377,6 @@
     <t>Cornelian cherry</t>
   </si>
   <si>
-    <t>Picea</t>
-  </si>
-  <si>
     <t>Spar</t>
   </si>
   <si>
@@ -1407,12 +1386,6 @@
     <t>Wilg</t>
   </si>
   <si>
-    <t>Salix</t>
-  </si>
-  <si>
-    <t>Crataegus</t>
-  </si>
-  <si>
     <t>Tilia cordata</t>
   </si>
   <si>
@@ -1456,6 +1429,162 @@
   </si>
   <si>
     <t>Acca sellowiana</t>
+  </si>
+  <si>
+    <t>Ziziphus jujuba</t>
+  </si>
+  <si>
+    <t>Phyllostachys sp.</t>
+  </si>
+  <si>
+    <t>Bamboo</t>
+  </si>
+  <si>
+    <t>Korean pine</t>
+  </si>
+  <si>
+    <t>Red mulberry</t>
+  </si>
+  <si>
+    <t>Black mulberry</t>
+  </si>
+  <si>
+    <t>Medlar</t>
+  </si>
+  <si>
+    <t>Leatherleaf mahonia</t>
+  </si>
+  <si>
+    <t>Whute mulberry</t>
+  </si>
+  <si>
+    <t>Goji berry</t>
+  </si>
+  <si>
+    <t>Daylily</t>
+  </si>
+  <si>
+    <t>Seaberry</t>
+  </si>
+  <si>
+    <t>Japanese raisin tree</t>
+  </si>
+  <si>
+    <t>Carolina silverbell</t>
+  </si>
+  <si>
+    <t>Liquorice</t>
+  </si>
+  <si>
+    <t>Chilean hazelnut</t>
+  </si>
+  <si>
+    <t>Citrus margarita</t>
+  </si>
+  <si>
+    <t>Kumquat</t>
+  </si>
+  <si>
+    <t>Fig</t>
+  </si>
+  <si>
+    <t>Alder buckthorn</t>
+  </si>
+  <si>
+    <t>Ebbing's Silverberry</t>
+  </si>
+  <si>
+    <t>Autumn olive</t>
+  </si>
+  <si>
+    <t>Loquat</t>
+  </si>
+  <si>
+    <t>Russian olive</t>
+  </si>
+  <si>
+    <t>Salix sp.</t>
+  </si>
+  <si>
+    <t>Picea sp.</t>
+  </si>
+  <si>
+    <t>Crataegus sp.</t>
+  </si>
+  <si>
+    <t>Persimmon</t>
+  </si>
+  <si>
+    <t>Persimmon 'Nikita's Gift'</t>
+  </si>
+  <si>
+    <t>Date-plum</t>
+  </si>
+  <si>
+    <t>Blue sausage fruit</t>
+  </si>
+  <si>
+    <t>C. cardunculus</t>
+  </si>
+  <si>
+    <t>Cardoon</t>
+  </si>
+  <si>
+    <t>Mandarin melon berry</t>
+  </si>
+  <si>
+    <t>Artichoke</t>
+  </si>
+  <si>
+    <t>Sweet chestnut</t>
+  </si>
+  <si>
+    <t>Japanese plum-yew</t>
+  </si>
+  <si>
+    <t>Chinese plum-yew</t>
+  </si>
+  <si>
+    <t>Siberian peashrub</t>
+  </si>
+  <si>
+    <t>Barberry</t>
+  </si>
+  <si>
+    <t>Silver birch</t>
+  </si>
+  <si>
+    <t>Paper mulberry</t>
+  </si>
+  <si>
+    <t>Chokeberry</t>
+  </si>
+  <si>
+    <t>Bearberry</t>
+  </si>
+  <si>
+    <t>Feijoa</t>
+  </si>
+  <si>
+    <t>Smooth serviceberry</t>
+  </si>
+  <si>
+    <t>Grey alder</t>
+  </si>
+  <si>
+    <t>Monkey puzzle tree</t>
+  </si>
+  <si>
+    <t>Prunus sp.</t>
+  </si>
+  <si>
+    <t>Wilde kers</t>
+  </si>
+  <si>
+    <t>Zoete kers (halfstam)</t>
+  </si>
+  <si>
+    <t>Zure kers (halfstam)</t>
   </si>
 </sst>
 </file>
@@ -1814,10 +1943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280D093D-8C82-4BD1-88A3-14D709597181}">
-  <dimension ref="A1:G126"/>
+  <dimension ref="A1:G127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B117" sqref="B117"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1833,39 +1962,39 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="B1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="F1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="G1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D2" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="E2">
         <v>3</v>
@@ -1879,13 +2008,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C3" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="D3" t="s">
+        <v>515</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -1896,7 +2028,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B4" t="s">
         <v>79</v>
@@ -1904,6 +2036,9 @@
       <c r="C4" t="s">
         <v>80</v>
       </c>
+      <c r="D4" t="s">
+        <v>80</v>
+      </c>
       <c r="E4">
         <v>2</v>
       </c>
@@ -1913,13 +2048,16 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C5" t="s">
-        <v>320</v>
+        <v>317</v>
+      </c>
+      <c r="D5" t="s">
+        <v>514</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -1930,7 +2068,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1938,6 +2076,9 @@
       <c r="C6" t="s">
         <v>19</v>
       </c>
+      <c r="D6" t="s">
+        <v>513</v>
+      </c>
       <c r="E6">
         <v>4</v>
       </c>
@@ -1950,16 +2091,16 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="B7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="D7" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E7">
         <v>2</v>
@@ -1970,13 +2111,16 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
       <c r="C8" t="s">
-        <v>321</v>
+        <v>318</v>
+      </c>
+      <c r="D8" t="s">
+        <v>512</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -1985,21 +2129,21 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D9" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="E9">
         <v>8</v>
@@ -2008,18 +2152,21 @@
         <v>8</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" t="s">
-        <v>159</v>
+        <v>157</v>
+      </c>
+      <c r="D10" t="s">
+        <v>511</v>
       </c>
       <c r="E10">
         <v>0.25</v>
@@ -2030,16 +2177,16 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B11" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="E11">
         <v>4</v>
@@ -2059,7 +2206,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>393</v>
+        <v>388</v>
+      </c>
+      <c r="D12" t="s">
+        <v>510</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -2073,13 +2223,16 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="B13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C13" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="D13" t="s">
+        <v>507</v>
       </c>
       <c r="E13">
         <v>2.5</v>
@@ -2090,13 +2243,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="D14" t="s">
+        <v>507</v>
       </c>
       <c r="E14">
         <v>2.5</v>
@@ -2105,18 +2261,21 @@
         <v>2.5</v>
       </c>
       <c r="G14" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>218</v>
+        <v>216</v>
+      </c>
+      <c r="D15" t="s">
+        <v>509</v>
       </c>
       <c r="E15">
         <v>12</v>
@@ -2127,13 +2286,16 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B16" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C16" t="s">
-        <v>194</v>
+        <v>192</v>
+      </c>
+      <c r="D16" t="s">
+        <v>508</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -2144,13 +2306,16 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="B17" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" t="s">
         <v>163</v>
       </c>
-      <c r="C17" t="s">
-        <v>165</v>
+      <c r="D17" t="s">
+        <v>507</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2159,21 +2324,21 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="B18" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="C18" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D18" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -2184,13 +2349,16 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C19" t="s">
-        <v>196</v>
+        <v>194</v>
+      </c>
+      <c r="D19" t="s">
+        <v>506</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2201,7 +2369,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B20" t="s">
         <v>96</v>
@@ -2210,7 +2378,7 @@
         <v>89</v>
       </c>
       <c r="D20" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E20">
         <v>6</v>
@@ -2221,16 +2389,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B21" t="s">
+        <v>217</v>
+      </c>
+      <c r="C21" t="s">
         <v>219</v>
       </c>
-      <c r="C21" t="s">
-        <v>221</v>
-      </c>
       <c r="D21" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="E21">
         <v>6</v>
@@ -2239,12 +2407,12 @@
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
         <v>94</v>
@@ -2253,7 +2421,7 @@
         <v>89</v>
       </c>
       <c r="D22" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E22">
         <v>10</v>
@@ -2264,16 +2432,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C23" t="s">
         <v>89</v>
       </c>
       <c r="D23" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="E23">
         <v>5</v>
@@ -2284,13 +2452,16 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B24" t="s">
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>467</v>
+        <v>458</v>
+      </c>
+      <c r="D24" t="s">
+        <v>445</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -2301,7 +2472,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="B25" t="s">
         <v>87</v>
@@ -2310,7 +2481,7 @@
         <v>89</v>
       </c>
       <c r="D25" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E25">
         <v>6</v>
@@ -2324,14 +2495,17 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C26" t="s">
         <v>69</v>
       </c>
+      <c r="D26" t="s">
+        <v>505</v>
+      </c>
       <c r="E26">
         <v>10</v>
       </c>
@@ -2341,13 +2515,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C27" t="s">
         <v>160</v>
       </c>
-      <c r="C27" t="s">
-        <v>162</v>
+      <c r="D27" t="s">
+        <v>504</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2356,21 +2533,21 @@
         <v>3</v>
       </c>
       <c r="G27" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="B28" t="s">
+        <v>140</v>
+      </c>
+      <c r="C28" t="s">
         <v>142</v>
       </c>
-      <c r="C28" t="s">
-        <v>144</v>
-      </c>
       <c r="D28" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E28">
         <v>30</v>
@@ -2379,21 +2556,21 @@
         <v>15</v>
       </c>
       <c r="G28" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B29" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C29" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D29" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E29">
         <v>2</v>
@@ -2402,12 +2579,12 @@
         <v>2</v>
       </c>
       <c r="G29" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -2416,7 +2593,7 @@
         <v>31</v>
       </c>
       <c r="D30" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="E30">
         <v>8</v>
@@ -2430,16 +2607,16 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="B31" t="s">
+        <v>143</v>
+      </c>
+      <c r="C31" t="s">
         <v>145</v>
       </c>
-      <c r="C31" t="s">
-        <v>147</v>
-      </c>
       <c r="D31" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -2448,12 +2625,12 @@
         <v>5</v>
       </c>
       <c r="G31" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B32" t="s">
         <v>93</v>
@@ -2462,7 +2639,7 @@
         <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E32">
         <v>6</v>
@@ -2473,16 +2650,16 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B33" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C33" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="D33" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E33">
         <v>6</v>
@@ -2493,7 +2670,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="B34" t="s">
         <v>90</v>
@@ -2502,7 +2679,7 @@
         <v>89</v>
       </c>
       <c r="D34" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E34">
         <v>9</v>
@@ -2516,16 +2693,16 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B35" t="s">
+        <v>166</v>
+      </c>
+      <c r="C35" t="s">
         <v>168</v>
       </c>
-      <c r="C35" t="s">
-        <v>170</v>
-      </c>
       <c r="D35" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -2534,21 +2711,21 @@
         <v>4</v>
       </c>
       <c r="G35" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="B36" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C36" t="s">
         <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E36">
         <v>6</v>
@@ -2557,21 +2734,21 @@
         <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
       <c r="B37" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E37">
         <v>7</v>
@@ -2582,7 +2759,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
@@ -2590,6 +2767,9 @@
       <c r="C38" t="s">
         <v>27</v>
       </c>
+      <c r="D38" t="s">
+        <v>503</v>
+      </c>
       <c r="E38">
         <v>20</v>
       </c>
@@ -2602,7 +2782,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="B39" t="s">
         <v>92</v>
@@ -2611,7 +2791,7 @@
         <v>89</v>
       </c>
       <c r="D39" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E39">
         <v>6</v>
@@ -2622,7 +2802,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="B40" t="s">
         <v>13</v>
@@ -2630,6 +2810,9 @@
       <c r="C40" t="s">
         <v>14</v>
       </c>
+      <c r="D40" t="s">
+        <v>502</v>
+      </c>
       <c r="E40">
         <v>1</v>
       </c>
@@ -2639,7 +2822,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B41" t="s">
         <v>74</v>
@@ -2648,7 +2831,7 @@
         <v>76</v>
       </c>
       <c r="D41" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -2662,7 +2845,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="B42" t="s">
         <v>95</v>
@@ -2671,7 +2854,7 @@
         <v>89</v>
       </c>
       <c r="D42" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E42">
         <v>10</v>
@@ -2682,13 +2865,16 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="B43" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" t="s">
         <v>121</v>
       </c>
-      <c r="C43" t="s">
-        <v>123</v>
+      <c r="D43" t="s">
+        <v>501</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -2697,21 +2883,21 @@
         <v>6</v>
       </c>
       <c r="G43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B44" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C44" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="D44" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="E44">
         <v>1.5</v>
@@ -2720,12 +2906,12 @@
         <v>1.5</v>
       </c>
       <c r="G44" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>376</v>
+        <v>499</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -2733,6 +2919,9 @@
       <c r="C45" t="s">
         <v>16</v>
       </c>
+      <c r="D45" t="s">
+        <v>500</v>
+      </c>
       <c r="E45">
         <v>1</v>
       </c>
@@ -2742,16 +2931,16 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
       <c r="B46" t="s">
-        <v>461</v>
+        <v>494</v>
       </c>
       <c r="C46" t="s">
         <v>89</v>
       </c>
       <c r="D46" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -2762,13 +2951,16 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B47" t="s">
         <v>84</v>
       </c>
       <c r="C47" t="s">
-        <v>387</v>
+        <v>382</v>
+      </c>
+      <c r="D47" t="s">
+        <v>498</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -2779,7 +2971,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B48" t="s">
         <v>85</v>
@@ -2787,6 +2979,9 @@
       <c r="C48" t="s">
         <v>86</v>
       </c>
+      <c r="D48" t="s">
+        <v>497</v>
+      </c>
       <c r="E48">
         <v>10</v>
       </c>
@@ -2796,13 +2991,16 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B49" t="s">
+        <v>125</v>
+      </c>
+      <c r="C49" t="s">
         <v>127</v>
       </c>
-      <c r="C49" t="s">
-        <v>129</v>
+      <c r="D49" t="s">
+        <v>496</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -2811,18 +3009,21 @@
         <v>8</v>
       </c>
       <c r="G49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B50" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" t="s">
         <v>124</v>
       </c>
-      <c r="C50" t="s">
-        <v>126</v>
+      <c r="D50" t="s">
+        <v>495</v>
       </c>
       <c r="E50">
         <v>15</v>
@@ -2831,12 +3032,12 @@
         <v>10</v>
       </c>
       <c r="G50" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="B51" t="s">
         <v>103</v>
@@ -2844,6 +3045,9 @@
       <c r="C51" t="s">
         <v>104</v>
       </c>
+      <c r="D51" t="s">
+        <v>491</v>
+      </c>
       <c r="E51">
         <v>3</v>
       </c>
@@ -2853,13 +3057,16 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="C52" t="s">
-        <v>386</v>
+        <v>490</v>
+      </c>
+      <c r="D52" t="s">
+        <v>490</v>
       </c>
       <c r="E52">
         <v>6</v>
@@ -2870,7 +3077,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B53" t="s">
         <v>97</v>
@@ -2879,7 +3086,7 @@
         <v>99</v>
       </c>
       <c r="D53" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="E53">
         <v>3</v>
@@ -2893,14 +3100,17 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B54" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="C54" t="s">
         <v>107</v>
       </c>
+      <c r="D54" t="s">
+        <v>489</v>
+      </c>
       <c r="E54">
         <v>5</v>
       </c>
@@ -2910,13 +3120,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="B55" t="s">
+        <v>208</v>
+      </c>
+      <c r="C55" t="s">
         <v>210</v>
       </c>
-      <c r="C55" t="s">
-        <v>212</v>
+      <c r="D55" t="s">
+        <v>488</v>
       </c>
       <c r="E55">
         <v>3</v>
@@ -2925,18 +3138,21 @@
         <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="B56" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C56" t="s">
-        <v>206</v>
+        <v>204</v>
+      </c>
+      <c r="D56" t="s">
+        <v>487</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -2947,13 +3163,16 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B57" t="s">
         <v>32</v>
       </c>
       <c r="C57" t="s">
-        <v>322</v>
+        <v>319</v>
+      </c>
+      <c r="D57" t="s">
+        <v>486</v>
       </c>
       <c r="E57">
         <v>6</v>
@@ -2967,16 +3186,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="B58" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="C58" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D58" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="E58">
         <v>14</v>
@@ -2987,13 +3206,16 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>171</v>
+      </c>
+      <c r="D59" t="s">
+        <v>485</v>
       </c>
       <c r="E59">
         <v>2.5</v>
@@ -3004,13 +3226,16 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="B60" t="s">
+        <v>172</v>
+      </c>
+      <c r="C60" t="s">
         <v>174</v>
       </c>
-      <c r="C60" t="s">
-        <v>176</v>
+      <c r="D60" t="s">
+        <v>484</v>
       </c>
       <c r="E60">
         <v>2.5</v>
@@ -3019,18 +3244,21 @@
         <v>2</v>
       </c>
       <c r="G60" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C61" t="s">
-        <v>192</v>
+        <v>190</v>
+      </c>
+      <c r="D61" t="s">
+        <v>483</v>
       </c>
       <c r="E61">
         <v>10</v>
@@ -3041,16 +3269,16 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="B62" t="s">
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D62" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="E62">
         <v>1.5</v>
@@ -3061,16 +3289,16 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C63" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D63" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E63">
         <v>20</v>
@@ -3081,7 +3309,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B64" t="s">
         <v>70</v>
@@ -3089,6 +3317,9 @@
       <c r="C64" t="s">
         <v>71</v>
       </c>
+      <c r="D64" t="s">
+        <v>482</v>
+      </c>
       <c r="E64">
         <v>1.5</v>
       </c>
@@ -3098,7 +3329,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="B65" t="s">
         <v>34</v>
@@ -3106,6 +3337,9 @@
       <c r="C65" t="s">
         <v>35</v>
       </c>
+      <c r="D65" t="s">
+        <v>481</v>
+      </c>
       <c r="E65">
         <v>6</v>
       </c>
@@ -3115,13 +3349,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B66" t="s">
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>471</v>
+        <v>462</v>
+      </c>
+      <c r="D66" t="s">
+        <v>480</v>
       </c>
       <c r="E66">
         <v>10</v>
@@ -3132,13 +3369,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
         <v>197</v>
       </c>
-      <c r="C67" t="s">
-        <v>199</v>
+      <c r="D67" t="s">
+        <v>479</v>
       </c>
       <c r="E67">
         <v>6</v>
@@ -3147,7 +3387,7 @@
         <v>5</v>
       </c>
       <c r="G67" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3160,6 +3400,9 @@
       <c r="C68" t="s">
         <v>12</v>
       </c>
+      <c r="D68" t="s">
+        <v>478</v>
+      </c>
       <c r="E68">
         <v>0.5</v>
       </c>
@@ -3169,16 +3412,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="B69" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C69" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="D69" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="E69">
         <v>30</v>
@@ -3189,13 +3432,16 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="B70" t="s">
+        <v>177</v>
+      </c>
+      <c r="C70" t="s">
         <v>179</v>
       </c>
-      <c r="C70" t="s">
-        <v>181</v>
+      <c r="D70" t="s">
+        <v>477</v>
       </c>
       <c r="E70">
         <v>2.5</v>
@@ -3204,18 +3450,21 @@
         <v>2.5</v>
       </c>
       <c r="G70" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="B71" t="s">
+        <v>128</v>
+      </c>
+      <c r="C71" t="s">
         <v>130</v>
       </c>
-      <c r="C71" t="s">
-        <v>132</v>
+      <c r="D71" t="s">
+        <v>476</v>
       </c>
       <c r="E71">
         <v>15</v>
@@ -3224,18 +3473,21 @@
         <v>12</v>
       </c>
       <c r="G71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B72" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="C72" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+      <c r="D72" t="s">
+        <v>207</v>
       </c>
       <c r="E72">
         <v>10</v>
@@ -3249,13 +3501,16 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C73" t="s">
-        <v>209</v>
+        <v>207</v>
+      </c>
+      <c r="D73" t="s">
+        <v>475</v>
       </c>
       <c r="E73">
         <v>10</v>
@@ -3266,7 +3521,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B74" t="s">
         <v>100</v>
@@ -3274,6 +3529,9 @@
       <c r="C74" t="s">
         <v>102</v>
       </c>
+      <c r="D74" t="s">
+        <v>474</v>
+      </c>
       <c r="E74">
         <v>5</v>
       </c>
@@ -3286,13 +3544,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B75" t="s">
+        <v>134</v>
+      </c>
+      <c r="C75" t="s">
         <v>136</v>
       </c>
-      <c r="C75" t="s">
-        <v>138</v>
+      <c r="D75" t="s">
+        <v>473</v>
       </c>
       <c r="E75">
         <v>8</v>
@@ -3301,21 +3562,21 @@
         <v>12</v>
       </c>
       <c r="G75" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
+        <v>336</v>
+      </c>
+      <c r="B76" t="s">
         <v>339</v>
       </c>
-      <c r="B76" t="s">
-        <v>342</v>
-      </c>
       <c r="C76" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="D76" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E76">
         <v>3</v>
@@ -3326,13 +3587,16 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="B77" t="s">
+        <v>131</v>
+      </c>
+      <c r="C77" t="s">
         <v>133</v>
       </c>
-      <c r="C77" t="s">
-        <v>135</v>
+      <c r="D77" t="s">
+        <v>472</v>
       </c>
       <c r="E77">
         <v>15</v>
@@ -3341,21 +3605,21 @@
         <v>10</v>
       </c>
       <c r="G77" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="B78" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="C78" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D78" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="E78">
         <v>6</v>
@@ -3366,16 +3630,16 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>281</v>
+        <v>516</v>
       </c>
       <c r="B79" t="s">
-        <v>108</v>
+        <v>516</v>
       </c>
       <c r="C79" t="s">
-        <v>110</v>
+        <v>517</v>
       </c>
       <c r="D79" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="E79">
         <v>6</v>
@@ -3383,108 +3647,108 @@
       <c r="F79">
         <v>4</v>
       </c>
-      <c r="G79" t="s">
-        <v>109</v>
-      </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B80" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>120</v>
+        <v>518</v>
       </c>
       <c r="D80" t="s">
-        <v>453</v>
+        <v>326</v>
       </c>
       <c r="E80">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F80">
         <v>4</v>
       </c>
       <c r="G80" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B81" t="s">
-        <v>1</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
-        <v>388</v>
+        <v>519</v>
       </c>
       <c r="D81" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="E81">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F81">
-        <v>6</v>
+        <v>4</v>
+      </c>
+      <c r="G81" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B82" t="s">
-        <v>111</v>
+        <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>470</v>
+        <v>383</v>
       </c>
       <c r="D82" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
       <c r="E82">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F82">
-        <v>3</v>
-      </c>
-      <c r="G82" t="s">
-        <v>112</v>
+        <v>6</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="B83" t="s">
-        <v>36</v>
+        <v>110</v>
       </c>
       <c r="C83" t="s">
-        <v>38</v>
+        <v>461</v>
+      </c>
+      <c r="D83" t="s">
+        <v>448</v>
       </c>
       <c r="E83">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F83">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G83" t="s">
-        <v>37</v>
+        <v>111</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
-        <v>155</v>
+        <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>331</v>
+        <v>471</v>
       </c>
       <c r="E84">
         <v>20</v>
@@ -3493,81 +3757,87 @@
         <v>15</v>
       </c>
       <c r="G84" t="s">
-        <v>154</v>
+        <v>37</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="B85" t="s">
-        <v>225</v>
+        <v>151</v>
       </c>
       <c r="C85" t="s">
-        <v>225</v>
+        <v>153</v>
       </c>
       <c r="D85" t="s">
-        <v>225</v>
+        <v>328</v>
       </c>
       <c r="E85">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="F85">
-        <v>3</v>
+        <v>15</v>
+      </c>
+      <c r="G85" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B86" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C86" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D86" t="s">
-        <v>365</v>
+        <v>222</v>
       </c>
       <c r="E86">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F86">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B87" t="s">
-        <v>464</v>
+        <v>223</v>
       </c>
       <c r="C87" t="s">
-        <v>116</v>
+        <v>224</v>
       </c>
       <c r="D87" t="s">
-        <v>451</v>
+        <v>362</v>
       </c>
       <c r="E87">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F87">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>223</v>
+        <v>286</v>
       </c>
       <c r="B88" t="s">
-        <v>223</v>
+        <v>455</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>115</v>
+      </c>
+      <c r="D88" t="s">
+        <v>445</v>
       </c>
       <c r="E88">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F88">
         <v>6</v>
@@ -3575,291 +3845,288 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
       <c r="B89" t="s">
-        <v>456</v>
+        <v>469</v>
       </c>
       <c r="C89" t="s">
-        <v>457</v>
+        <v>221</v>
       </c>
       <c r="D89" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E89">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="F89">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>290</v>
+        <v>493</v>
       </c>
       <c r="B90" t="s">
-        <v>150</v>
+        <v>493</v>
       </c>
       <c r="C90" t="s">
-        <v>151</v>
+        <v>450</v>
       </c>
       <c r="D90" t="s">
-        <v>449</v>
+        <v>459</v>
       </c>
       <c r="E90">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F90">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>473</v>
+        <v>287</v>
       </c>
       <c r="B91" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="C91" t="s">
-        <v>436</v>
+        <v>149</v>
       </c>
       <c r="D91" t="s">
-        <v>435</v>
+        <v>443</v>
       </c>
       <c r="E91">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F91">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>474</v>
+        <v>464</v>
       </c>
       <c r="B92" t="s">
-        <v>475</v>
+        <v>50</v>
       </c>
       <c r="C92" t="s">
-        <v>185</v>
+        <v>430</v>
       </c>
       <c r="D92" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E92">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F92">
         <v>3</v>
       </c>
-      <c r="G92" t="s">
-        <v>184</v>
-      </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>291</v>
+        <v>465</v>
       </c>
       <c r="B93" t="s">
-        <v>39</v>
+        <v>466</v>
       </c>
       <c r="C93" t="s">
-        <v>389</v>
+        <v>183</v>
       </c>
       <c r="D93" t="s">
-        <v>448</v>
+        <v>428</v>
       </c>
       <c r="E93">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F93">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="G93" t="s">
-        <v>40</v>
+        <v>182</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="B94" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
-        <v>44</v>
+        <v>384</v>
       </c>
       <c r="D94" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="E94">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F94">
-        <v>2</v>
+        <v>1.5</v>
+      </c>
+      <c r="G94" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B95" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C95" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D95" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="E95">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F95">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B96" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="C96" t="s">
-        <v>437</v>
+        <v>42</v>
       </c>
       <c r="D96" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="E96">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F96">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>369</v>
+        <v>291</v>
       </c>
       <c r="B97" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>354</v>
+        <v>431</v>
       </c>
       <c r="D97" t="s">
-        <v>353</v>
+        <v>432</v>
       </c>
       <c r="E97">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F97">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>295</v>
+        <v>366</v>
       </c>
       <c r="B98" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C98" t="s">
-        <v>47</v>
+        <v>351</v>
       </c>
       <c r="D98" t="s">
-        <v>327</v>
+        <v>350</v>
       </c>
       <c r="E98">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="F98">
-        <v>1.5</v>
-      </c>
-      <c r="G98" t="s">
-        <v>46</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="B99" t="s">
-        <v>182</v>
+        <v>45</v>
       </c>
       <c r="C99" t="s">
-        <v>444</v>
+        <v>47</v>
       </c>
       <c r="D99" t="s">
-        <v>443</v>
+        <v>324</v>
       </c>
       <c r="E99">
-        <v>1.25</v>
+        <v>2</v>
       </c>
       <c r="F99">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="G99" t="s">
-        <v>183</v>
+        <v>46</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>392</v>
+        <v>293</v>
       </c>
       <c r="B100" t="s">
-        <v>51</v>
+        <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>52</v>
+        <v>438</v>
       </c>
       <c r="D100" t="s">
-        <v>352</v>
+        <v>437</v>
       </c>
       <c r="E100">
-        <v>2</v>
+        <v>1.25</v>
       </c>
       <c r="F100">
-        <v>2</v>
+        <v>1.25</v>
+      </c>
+      <c r="G100" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>297</v>
+        <v>387</v>
       </c>
       <c r="B101" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C101" t="s">
-        <v>442</v>
+        <v>52</v>
       </c>
       <c r="D101" t="s">
-        <v>441</v>
+        <v>349</v>
       </c>
       <c r="E101">
         <v>2</v>
       </c>
       <c r="F101">
-        <v>1.5</v>
-      </c>
-      <c r="G101" t="s">
-        <v>49</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>370</v>
+        <v>294</v>
       </c>
       <c r="B102" t="s">
-        <v>200</v>
+        <v>48</v>
       </c>
       <c r="C102" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="D102" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E102">
         <v>2</v>
@@ -3868,428 +4135,431 @@
         <v>1.5</v>
       </c>
       <c r="G102" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>298</v>
+        <v>367</v>
       </c>
       <c r="B103" t="s">
-        <v>82</v>
+        <v>198</v>
       </c>
       <c r="C103" t="s">
-        <v>42</v>
+        <v>434</v>
       </c>
       <c r="D103" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="E103">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F103">
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G103" t="s">
-        <v>83</v>
+        <v>199</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>395</v>
+        <v>295</v>
       </c>
       <c r="B104" t="s">
-        <v>394</v>
+        <v>82</v>
       </c>
       <c r="C104" t="s">
-        <v>396</v>
+        <v>42</v>
       </c>
       <c r="D104" t="s">
-        <v>397</v>
+        <v>439</v>
       </c>
       <c r="E104">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="G104" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>368</v>
+        <v>390</v>
       </c>
       <c r="B105" t="s">
-        <v>203</v>
+        <v>389</v>
       </c>
       <c r="C105" t="s">
-        <v>204</v>
+        <v>391</v>
       </c>
       <c r="D105" t="s">
-        <v>433</v>
+        <v>392</v>
       </c>
       <c r="E105">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F105">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
+        <v>201</v>
       </c>
       <c r="C106" t="s">
-        <v>57</v>
+        <v>202</v>
       </c>
       <c r="D106" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E106">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="F106">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C107" t="s">
-        <v>430</v>
+        <v>57</v>
       </c>
       <c r="D107" t="s">
-        <v>452</v>
+        <v>425</v>
       </c>
       <c r="E107">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="F107">
-        <v>7</v>
-      </c>
-      <c r="G107" t="s">
-        <v>59</v>
+        <v>3</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B108" t="s">
-        <v>105</v>
+        <v>58</v>
       </c>
       <c r="C108" t="s">
-        <v>55</v>
+        <v>424</v>
       </c>
       <c r="D108" t="s">
-        <v>344</v>
+        <v>446</v>
       </c>
       <c r="E108">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="F108">
-        <v>2.5</v>
+        <v>7</v>
       </c>
       <c r="G108" t="s">
-        <v>106</v>
+        <v>59</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B109" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s">
-        <v>141</v>
+        <v>55</v>
       </c>
       <c r="D109" t="s">
-        <v>425</v>
+        <v>341</v>
       </c>
       <c r="E109">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F109">
-        <v>8</v>
+        <v>2.5</v>
       </c>
       <c r="G109" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B110" t="s">
-        <v>53</v>
+        <v>137</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>139</v>
       </c>
       <c r="D110" t="s">
-        <v>432</v>
+        <v>419</v>
       </c>
       <c r="E110">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="F110">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="G110" t="s">
-        <v>54</v>
+        <v>138</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="B111" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C111" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="D111" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="E111">
         <v>4</v>
       </c>
       <c r="F111">
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="G111" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="B112" t="s">
-        <v>2</v>
+        <v>61</v>
       </c>
       <c r="C112" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="D112" t="s">
-        <v>333</v>
+        <v>418</v>
       </c>
       <c r="E112">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="F112">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B113" t="s">
-        <v>188</v>
+        <v>2</v>
       </c>
       <c r="C113" t="s">
-        <v>190</v>
+        <v>3</v>
       </c>
       <c r="D113" t="s">
-        <v>423</v>
+        <v>330</v>
       </c>
       <c r="E113">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F113">
-        <v>3</v>
-      </c>
-      <c r="G113" t="s">
-        <v>189</v>
+        <v>8</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>460</v>
+        <v>303</v>
       </c>
       <c r="B114" t="s">
-        <v>460</v>
+        <v>186</v>
       </c>
       <c r="C114" t="s">
-        <v>459</v>
+        <v>188</v>
       </c>
       <c r="D114" t="s">
-        <v>458</v>
+        <v>417</v>
       </c>
       <c r="E114">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="F114">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="G114" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>307</v>
+        <v>492</v>
       </c>
       <c r="B115" t="s">
-        <v>426</v>
+        <v>492</v>
       </c>
       <c r="C115" t="s">
-        <v>429</v>
+        <v>452</v>
       </c>
       <c r="D115" t="s">
-        <v>428</v>
+        <v>451</v>
       </c>
       <c r="E115">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F115">
-        <v>5</v>
-      </c>
-      <c r="G115" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>463</v>
+        <v>304</v>
       </c>
       <c r="B116" t="s">
-        <v>462</v>
+        <v>420</v>
       </c>
       <c r="C116" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="D116" t="s">
         <v>422</v>
       </c>
       <c r="E116">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="F116">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="G116" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>308</v>
+        <v>454</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>453</v>
       </c>
       <c r="C117" t="s">
-        <v>6</v>
+        <v>414</v>
       </c>
       <c r="D117" t="s">
-        <v>345</v>
+        <v>416</v>
       </c>
       <c r="E117">
-        <v>20</v>
+        <v>3</v>
       </c>
       <c r="F117">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B118" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C118" t="s">
-        <v>421</v>
+        <v>6</v>
       </c>
       <c r="D118" t="s">
-        <v>419</v>
+        <v>342</v>
       </c>
       <c r="E118">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="F118">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B119" t="s">
-        <v>72</v>
+        <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>73</v>
+        <v>415</v>
       </c>
       <c r="D119" t="s">
-        <v>72</v>
+        <v>413</v>
       </c>
       <c r="E119">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F119">
-        <v>1.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>418</v>
+        <v>307</v>
       </c>
       <c r="B120" t="s">
-        <v>417</v>
+        <v>72</v>
       </c>
       <c r="C120" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D120" t="s">
-        <v>416</v>
+        <v>72</v>
       </c>
       <c r="E120">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="F120">
-        <v>0.5</v>
-      </c>
-      <c r="G120" t="s">
-        <v>77</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>358</v>
+        <v>412</v>
       </c>
       <c r="B121" t="s">
-        <v>156</v>
+        <v>411</v>
       </c>
       <c r="C121" t="s">
-        <v>361</v>
+        <v>78</v>
       </c>
       <c r="D121" t="s">
-        <v>362</v>
+        <v>410</v>
       </c>
       <c r="E121">
         <v>0.5</v>
       </c>
       <c r="F121">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="G121" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B122" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C122" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D122" t="s">
         <v>359</v>
       </c>
       <c r="E122">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -4297,93 +4567,113 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>311</v>
+        <v>354</v>
       </c>
       <c r="B123" t="s">
-        <v>410</v>
+        <v>155</v>
       </c>
       <c r="C123" t="s">
-        <v>409</v>
+        <v>357</v>
       </c>
       <c r="D123" t="s">
-        <v>409</v>
+        <v>356</v>
       </c>
       <c r="E123">
-        <v>10</v>
+        <v>0.2</v>
       </c>
       <c r="F123">
-        <v>7</v>
-      </c>
-      <c r="G123" t="s">
-        <v>117</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="B124" t="s">
-        <v>63</v>
+        <v>468</v>
       </c>
       <c r="C124" t="s">
-        <v>64</v>
+        <v>404</v>
       </c>
       <c r="D124" t="s">
-        <v>328</v>
+        <v>404</v>
       </c>
       <c r="E124">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="F124">
-        <v>1.5</v>
+        <v>7</v>
+      </c>
+      <c r="G124" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B125" t="s">
-        <v>7</v>
+        <v>63</v>
       </c>
       <c r="C125" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D125" t="s">
-        <v>351</v>
+        <v>325</v>
       </c>
       <c r="E125">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F125">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>310</v>
+      </c>
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>8</v>
+      </c>
+      <c r="D126" t="s">
+        <v>348</v>
+      </c>
+      <c r="E126">
+        <v>2.5</v>
+      </c>
+      <c r="F126">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
         <v>65</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B127" t="s">
         <v>65</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C127" t="s">
         <v>67</v>
       </c>
-      <c r="D126" t="s">
-        <v>415</v>
-      </c>
-      <c r="E126">
+      <c r="D127" t="s">
+        <v>409</v>
+      </c>
+      <c r="E127">
         <v>2</v>
       </c>
-      <c r="F126">
+      <c r="F127">
         <v>2</v>
       </c>
-      <c r="G126" t="s">
+      <c r="G127" t="s">
         <v>66</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G126">
-    <sortCondition ref="A2:A126"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G127">
+    <sortCondition ref="A2:A127"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Added jasmine and oak
</commit_message>
<xml_diff>
--- a/scripts/voedselbos_species.xlsx
+++ b/scripts/voedselbos_species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{651B2011-4676-482A-A105-671990386CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97F2B245-ACC6-4B14-B3B9-A39F1C712DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29010" yWindow="1980" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="528">
   <si>
     <t>Hovenia dulcis</t>
   </si>
@@ -1585,6 +1585,30 @@
   </si>
   <si>
     <t>Zure kers (halfstam)</t>
+  </si>
+  <si>
+    <t>J. officinale</t>
+  </si>
+  <si>
+    <t>Jasminum officinale</t>
+  </si>
+  <si>
+    <t>Common jasmine</t>
+  </si>
+  <si>
+    <t>Zomerjasmijn</t>
+  </si>
+  <si>
+    <t>Q. robur</t>
+  </si>
+  <si>
+    <t>Quercus robur</t>
+  </si>
+  <si>
+    <t>Zomereik</t>
+  </si>
+  <si>
+    <t>Common oak</t>
   </si>
 </sst>
 </file>
@@ -1943,10 +1967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280D093D-8C82-4BD1-88A3-14D709597181}">
-  <dimension ref="A1:G127"/>
+  <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4671,6 +4695,46 @@
         <v>66</v>
       </c>
     </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>520</v>
+      </c>
+      <c r="B128" t="s">
+        <v>521</v>
+      </c>
+      <c r="C128" t="s">
+        <v>523</v>
+      </c>
+      <c r="D128" t="s">
+        <v>522</v>
+      </c>
+      <c r="E128">
+        <v>2</v>
+      </c>
+      <c r="F128">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>524</v>
+      </c>
+      <c r="B129" t="s">
+        <v>525</v>
+      </c>
+      <c r="C129" t="s">
+        <v>526</v>
+      </c>
+      <c r="D129" t="s">
+        <v>527</v>
+      </c>
+      <c r="E129">
+        <v>6</v>
+      </c>
+      <c r="F129">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G127">
     <sortCondition ref="A2:A127"/>

</xml_diff>

<commit_message>
Version bump and updates species name
</commit_message>
<xml_diff>
--- a/scripts/voedselbos_species.xlsx
+++ b/scripts/voedselbos_species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\damien\bosmapper\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77AD93A-BF78-4553-AE34-08A1E35587BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DCEB7F-6ADE-4002-BCCA-1529104BEFF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1905" windowWidth="29040" windowHeight="15990" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
+    <workbookView xWindow="29010" yWindow="1980" windowWidth="26595" windowHeight="11985" xr2:uid="{41C94313-E097-42C3-9518-1AB02B51329D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1179,9 +1179,6 @@
     <t>Peer (hoogstam)</t>
   </si>
   <si>
-    <t>Fluweelboom (klein)</t>
-  </si>
-  <si>
     <t>Salal</t>
   </si>
   <si>
@@ -1663,6 +1660,9 @@
   </si>
   <si>
     <t>Olijf</t>
+  </si>
+  <si>
+    <t>Welriekende sumak</t>
   </si>
 </sst>
 </file>
@@ -2023,8 +2023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280D093D-8C82-4BD1-88A3-14D709597181}">
   <dimension ref="A1:G134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="F135" sqref="F135"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2095,7 @@
         <v>214</v>
       </c>
       <c r="D3" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E3">
         <v>25</v>
@@ -2135,7 +2135,7 @@
         <v>317</v>
       </c>
       <c r="D5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E5">
         <v>15</v>
@@ -2155,7 +2155,7 @@
         <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -2192,13 +2192,13 @@
         <v>234</v>
       </c>
       <c r="B8" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C8" t="s">
         <v>318</v>
       </c>
       <c r="D8" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E8">
         <v>3</v>
@@ -2244,7 +2244,7 @@
         <v>157</v>
       </c>
       <c r="D10" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E10">
         <v>0.25</v>
@@ -2284,10 +2284,10 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D12" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E12">
         <v>3</v>
@@ -2310,7 +2310,7 @@
         <v>163</v>
       </c>
       <c r="D13" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E13">
         <v>2.5</v>
@@ -2330,7 +2330,7 @@
         <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E14">
         <v>2.5</v>
@@ -2353,7 +2353,7 @@
         <v>216</v>
       </c>
       <c r="D15" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E15">
         <v>12</v>
@@ -2373,7 +2373,7 @@
         <v>192</v>
       </c>
       <c r="D16" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E16">
         <v>20</v>
@@ -2393,7 +2393,7 @@
         <v>163</v>
       </c>
       <c r="D17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E17">
         <v>2</v>
@@ -2413,7 +2413,7 @@
         <v>364</v>
       </c>
       <c r="C18" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D18" t="s">
         <v>353</v>
@@ -2436,7 +2436,7 @@
         <v>194</v>
       </c>
       <c r="D19" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2536,10 +2536,10 @@
         <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="D24" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E24">
         <v>3</v>
@@ -2582,7 +2582,7 @@
         <v>69</v>
       </c>
       <c r="D26" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E26">
         <v>10</v>
@@ -2602,7 +2602,7 @@
         <v>160</v>
       </c>
       <c r="D27" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -2694,7 +2694,7 @@
         <v>145</v>
       </c>
       <c r="D31" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E31">
         <v>6</v>
@@ -2728,13 +2728,13 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>401</v>
+      </c>
+      <c r="B33" t="s">
+        <v>400</v>
+      </c>
+      <c r="C33" t="s">
         <v>402</v>
-      </c>
-      <c r="B33" t="s">
-        <v>401</v>
-      </c>
-      <c r="C33" t="s">
-        <v>403</v>
       </c>
       <c r="D33" t="s">
         <v>346</v>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B37" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
@@ -2846,7 +2846,7 @@
         <v>27</v>
       </c>
       <c r="D38" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E38">
         <v>20</v>
@@ -2889,7 +2889,7 @@
         <v>14</v>
       </c>
       <c r="D40" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -2952,7 +2952,7 @@
         <v>121</v>
       </c>
       <c r="D43" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E43">
         <v>6</v>
@@ -2989,7 +2989,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B45" t="s">
         <v>15</v>
@@ -2998,7 +2998,7 @@
         <v>16</v>
       </c>
       <c r="D45" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B46" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C46" t="s">
         <v>89</v>
@@ -3038,7 +3038,7 @@
         <v>382</v>
       </c>
       <c r="D47" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E47">
         <v>5</v>
@@ -3058,7 +3058,7 @@
         <v>86</v>
       </c>
       <c r="D48" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E48">
         <v>10</v>
@@ -3078,7 +3078,7 @@
         <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="E49">
         <v>15</v>
@@ -3101,7 +3101,7 @@
         <v>124</v>
       </c>
       <c r="D50" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E50">
         <v>15</v>
@@ -3124,7 +3124,7 @@
         <v>104</v>
       </c>
       <c r="D51" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E51">
         <v>3</v>
@@ -3138,13 +3138,13 @@
         <v>260</v>
       </c>
       <c r="B52" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C52" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D52" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="E52">
         <v>6</v>
@@ -3181,13 +3181,13 @@
         <v>371</v>
       </c>
       <c r="B54" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C54" t="s">
         <v>107</v>
       </c>
       <c r="D54" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E54">
         <v>5</v>
@@ -3207,7 +3207,7 @@
         <v>210</v>
       </c>
       <c r="D55" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E55">
         <v>3</v>
@@ -3230,7 +3230,7 @@
         <v>204</v>
       </c>
       <c r="D56" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="E56">
         <v>4</v>
@@ -3250,7 +3250,7 @@
         <v>319</v>
       </c>
       <c r="D57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="E57">
         <v>6</v>
@@ -3264,16 +3264,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B58" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C58" t="s">
+        <v>396</v>
+      </c>
+      <c r="D58" t="s">
         <v>397</v>
-      </c>
-      <c r="D58" t="s">
-        <v>398</v>
       </c>
       <c r="E58">
         <v>14</v>
@@ -3293,7 +3293,7 @@
         <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="E59">
         <v>2.5</v>
@@ -3313,7 +3313,7 @@
         <v>174</v>
       </c>
       <c r="D60" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E60">
         <v>2.5</v>
@@ -3336,7 +3336,7 @@
         <v>190</v>
       </c>
       <c r="D61" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E61">
         <v>10</v>
@@ -3353,10 +3353,10 @@
         <v>81</v>
       </c>
       <c r="C62" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D62" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E62">
         <v>1.5</v>
@@ -3396,7 +3396,7 @@
         <v>71</v>
       </c>
       <c r="D64" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="E64">
         <v>1.5</v>
@@ -3416,7 +3416,7 @@
         <v>35</v>
       </c>
       <c r="D65" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E65">
         <v>6</v>
@@ -3433,10 +3433,10 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D66" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E66">
         <v>10</v>
@@ -3456,7 +3456,7 @@
         <v>197</v>
       </c>
       <c r="D67" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E67">
         <v>6</v>
@@ -3479,7 +3479,7 @@
         <v>12</v>
       </c>
       <c r="D68" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E68">
         <v>0.5</v>
@@ -3490,16 +3490,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>393</v>
+      </c>
+      <c r="B69" t="s">
+        <v>392</v>
+      </c>
+      <c r="C69" t="s">
+        <v>395</v>
+      </c>
+      <c r="D69" t="s">
         <v>394</v>
-      </c>
-      <c r="B69" t="s">
-        <v>393</v>
-      </c>
-      <c r="C69" t="s">
-        <v>396</v>
-      </c>
-      <c r="D69" t="s">
-        <v>395</v>
       </c>
       <c r="E69">
         <v>30</v>
@@ -3519,7 +3519,7 @@
         <v>179</v>
       </c>
       <c r="D70" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="E70">
         <v>2.5</v>
@@ -3542,7 +3542,7 @@
         <v>130</v>
       </c>
       <c r="D71" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="E71">
         <v>15</v>
@@ -3588,7 +3588,7 @@
         <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="E73">
         <v>10</v>
@@ -3608,7 +3608,7 @@
         <v>102</v>
       </c>
       <c r="D74" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E74">
         <v>5</v>
@@ -3631,7 +3631,7 @@
         <v>136</v>
       </c>
       <c r="D75" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E75">
         <v>8</v>
@@ -3674,7 +3674,7 @@
         <v>133</v>
       </c>
       <c r="D77" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E77">
         <v>15</v>
@@ -3688,16 +3688,16 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>406</v>
+      </c>
+      <c r="B78" t="s">
+        <v>405</v>
+      </c>
+      <c r="C78" t="s">
+        <v>404</v>
+      </c>
+      <c r="D78" t="s">
         <v>407</v>
-      </c>
-      <c r="B78" t="s">
-        <v>406</v>
-      </c>
-      <c r="C78" t="s">
-        <v>405</v>
-      </c>
-      <c r="D78" t="s">
-        <v>408</v>
       </c>
       <c r="E78">
         <v>6</v>
@@ -3708,13 +3708,13 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>515</v>
+      </c>
+      <c r="B79" t="s">
+        <v>515</v>
+      </c>
+      <c r="C79" t="s">
         <v>516</v>
-      </c>
-      <c r="B79" t="s">
-        <v>516</v>
-      </c>
-      <c r="C79" t="s">
-        <v>517</v>
       </c>
       <c r="D79" t="s">
         <v>326</v>
@@ -3734,7 +3734,7 @@
         <v>108</v>
       </c>
       <c r="C80" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D80" t="s">
         <v>326</v>
@@ -3757,10 +3757,10 @@
         <v>117</v>
       </c>
       <c r="C81" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D81" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="E81">
         <v>4</v>
@@ -3783,7 +3783,7 @@
         <v>383</v>
       </c>
       <c r="D82" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="E82">
         <v>10</v>
@@ -3800,10 +3800,10 @@
         <v>110</v>
       </c>
       <c r="C83" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D83" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E83">
         <v>4</v>
@@ -3826,7 +3826,7 @@
         <v>38</v>
       </c>
       <c r="D84" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E84">
         <v>20</v>
@@ -3906,13 +3906,13 @@
         <v>286</v>
       </c>
       <c r="B88" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C88" t="s">
         <v>115</v>
       </c>
       <c r="D88" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="E88">
         <v>7</v>
@@ -3923,16 +3923,16 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B89" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C89" t="s">
         <v>221</v>
       </c>
       <c r="D89" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E89">
         <v>6</v>
@@ -3943,16 +3943,16 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B90" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C90" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D90" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E90">
         <v>14</v>
@@ -3972,7 +3972,7 @@
         <v>149</v>
       </c>
       <c r="D91" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="E91">
         <v>15</v>
@@ -3983,16 +3983,16 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B92" t="s">
         <v>50</v>
       </c>
       <c r="C92" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D92" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="E92">
         <v>2</v>
@@ -4003,16 +4003,16 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
+        <v>464</v>
+      </c>
+      <c r="B93" t="s">
         <v>465</v>
-      </c>
-      <c r="B93" t="s">
-        <v>466</v>
       </c>
       <c r="C93" t="s">
         <v>183</v>
       </c>
       <c r="D93" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="E93">
         <v>3</v>
@@ -4032,10 +4032,10 @@
         <v>39</v>
       </c>
       <c r="C94" t="s">
-        <v>384</v>
+        <v>545</v>
       </c>
       <c r="D94" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="E94">
         <v>1.5</v>
@@ -4058,7 +4058,7 @@
         <v>44</v>
       </c>
       <c r="D95" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E95">
         <v>2</v>
@@ -4078,7 +4078,7 @@
         <v>42</v>
       </c>
       <c r="D96" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="E96">
         <v>3</v>
@@ -4095,10 +4095,10 @@
         <v>9</v>
       </c>
       <c r="C97" t="s">
+        <v>430</v>
+      </c>
+      <c r="D97" t="s">
         <v>431</v>
-      </c>
-      <c r="D97" t="s">
-        <v>432</v>
       </c>
       <c r="E97">
         <v>1</v>
@@ -4158,10 +4158,10 @@
         <v>180</v>
       </c>
       <c r="C100" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D100" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E100">
         <v>1.25</v>
@@ -4175,7 +4175,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B101" t="s">
         <v>51</v>
@@ -4201,10 +4201,10 @@
         <v>48</v>
       </c>
       <c r="C102" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D102" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="E102">
         <v>2</v>
@@ -4224,10 +4224,10 @@
         <v>198</v>
       </c>
       <c r="C103" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="D103" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="E103">
         <v>2</v>
@@ -4250,7 +4250,7 @@
         <v>42</v>
       </c>
       <c r="D104" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E104">
         <v>3</v>
@@ -4264,16 +4264,16 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>389</v>
+      </c>
+      <c r="B105" t="s">
+        <v>388</v>
+      </c>
+      <c r="C105" t="s">
         <v>390</v>
       </c>
-      <c r="B105" t="s">
-        <v>389</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="D105" t="s">
         <v>391</v>
-      </c>
-      <c r="D105" t="s">
-        <v>392</v>
       </c>
       <c r="E105">
         <v>1</v>
@@ -4293,7 +4293,7 @@
         <v>202</v>
       </c>
       <c r="D106" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E106">
         <v>15</v>
@@ -4313,7 +4313,7 @@
         <v>57</v>
       </c>
       <c r="D107" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="E107">
         <v>4</v>
@@ -4330,10 +4330,10 @@
         <v>58</v>
       </c>
       <c r="C108" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D108" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E108">
         <v>12</v>
@@ -4379,7 +4379,7 @@
         <v>139</v>
       </c>
       <c r="D110" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E110">
         <v>20</v>
@@ -4402,7 +4402,7 @@
         <v>55</v>
       </c>
       <c r="D111" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="E111">
         <v>4</v>
@@ -4425,7 +4425,7 @@
         <v>62</v>
       </c>
       <c r="D112" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E112">
         <v>4</v>
@@ -4465,7 +4465,7 @@
         <v>188</v>
       </c>
       <c r="D114" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E114">
         <v>3</v>
@@ -4479,16 +4479,16 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B115" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C115" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D115" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E115">
         <v>10</v>
@@ -4502,13 +4502,13 @@
         <v>304</v>
       </c>
       <c r="B116" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C116" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D116" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E116">
         <v>7</v>
@@ -4522,16 +4522,16 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B117" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C117" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D117" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E117">
         <v>3</v>
@@ -4568,10 +4568,10 @@
         <v>4</v>
       </c>
       <c r="C119" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D119" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E119">
         <v>3</v>
@@ -4602,16 +4602,16 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B121" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C121" t="s">
         <v>78</v>
       </c>
       <c r="D121" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E121">
         <v>0.5</v>
@@ -4668,13 +4668,13 @@
         <v>308</v>
       </c>
       <c r="B124" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C124" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D124" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E124">
         <v>10</v>
@@ -4737,7 +4737,7 @@
         <v>67</v>
       </c>
       <c r="D127" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E127">
         <v>2</v>
@@ -4751,16 +4751,16 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>519</v>
+      </c>
+      <c r="B128" t="s">
         <v>520</v>
       </c>
-      <c r="B128" t="s">
+      <c r="C128" t="s">
+        <v>522</v>
+      </c>
+      <c r="D128" t="s">
         <v>521</v>
-      </c>
-      <c r="C128" t="s">
-        <v>523</v>
-      </c>
-      <c r="D128" t="s">
-        <v>522</v>
       </c>
       <c r="E128">
         <v>2</v>
@@ -4771,16 +4771,16 @@
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
+        <v>523</v>
+      </c>
+      <c r="B129" t="s">
         <v>524</v>
       </c>
-      <c r="B129" t="s">
+      <c r="C129" t="s">
         <v>525</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
         <v>526</v>
-      </c>
-      <c r="D129" t="s">
-        <v>527</v>
       </c>
       <c r="E129">
         <v>6</v>
@@ -4791,16 +4791,16 @@
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B130" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C130" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D130" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E130">
         <v>1.5</v>
@@ -4811,16 +4811,16 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B131" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C131" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D131" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E131">
         <v>1</v>
@@ -4831,16 +4831,16 @@
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
+        <v>534</v>
+      </c>
+      <c r="B132" t="s">
+        <v>533</v>
+      </c>
+      <c r="C132" t="s">
+        <v>536</v>
+      </c>
+      <c r="D132" t="s">
         <v>535</v>
-      </c>
-      <c r="B132" t="s">
-        <v>534</v>
-      </c>
-      <c r="C132" t="s">
-        <v>537</v>
-      </c>
-      <c r="D132" t="s">
-        <v>536</v>
       </c>
       <c r="E132">
         <v>2</v>
@@ -4851,16 +4851,16 @@
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>538</v>
+      </c>
+      <c r="B133" t="s">
+        <v>537</v>
+      </c>
+      <c r="C133" t="s">
+        <v>540</v>
+      </c>
+      <c r="D133" t="s">
         <v>539</v>
-      </c>
-      <c r="B133" t="s">
-        <v>538</v>
-      </c>
-      <c r="C133" t="s">
-        <v>541</v>
-      </c>
-      <c r="D133" t="s">
-        <v>540</v>
       </c>
       <c r="E133">
         <v>1</v>
@@ -4871,16 +4871,16 @@
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
+        <v>542</v>
+      </c>
+      <c r="B134" t="s">
+        <v>541</v>
+      </c>
+      <c r="C134" t="s">
+        <v>544</v>
+      </c>
+      <c r="D134" t="s">
         <v>543</v>
-      </c>
-      <c r="B134" t="s">
-        <v>542</v>
-      </c>
-      <c r="C134" t="s">
-        <v>545</v>
-      </c>
-      <c r="D134" t="s">
-        <v>544</v>
       </c>
       <c r="E134">
         <v>4</v>

</xml_diff>